<commit_message>
Added the index for the bert score stats file
</commit_message>
<xml_diff>
--- a/Testing Model in the Loop/ML_datasets_BERTScore_stats.xlsx
+++ b/Testing Model in the Loop/ML_datasets_BERTScore_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,30 +434,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>BERTScore_Human Classifications vs Llama2 Simple Conclusion Category</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>BERTScore_Human Classifications vs Mistral Simple Conclusion Category</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>BERTScore_Human Extracted Arguments vs LLama2 Extracted Arguments</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>BERTScore_Human Extracted Arguments vs Mistral Extracted Arguments</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>236</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>236</v>
@@ -468,102 +470,140 @@
       <c r="D2" t="n">
         <v>236</v>
       </c>
+      <c r="E2" t="n">
+        <v>236</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>0.8973926749017279</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>0.9139234644629187</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.877872622366679</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.8916541897391869</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0.1144876811105954</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>0.1271092663810594</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.1054802715989092</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.1552294298292282</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0.3922216594219208</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>0.445945143699646</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.4882096648216248</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.3893436193466187</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>0.8554607033729553</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0.8699711859226227</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0.8684156388044357</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.8941315561532974</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>0.8973172307014465</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>0.9999998807907104</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>0.9095499813556671</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.9591342210769653</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0.9999998807907104</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>0.9999998807907104</v>
       </c>
       <c r="C8" t="n">
+        <v>0.9999998807907104</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.9423744231462479</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>0.9830563217401505</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>0.9999999403953552</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>0.9836103916168213</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>